<commit_message>
pdf and xlsx buttons working with frontend and backend
</commit_message>
<xml_diff>
--- a/backend/spotify_export.xlsx
+++ b/backend/spotify_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,21 +475,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>KETTAMA</t>
+          <t>Kalyma</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Yosemite - Philip George Remix</t>
+          <t>SACROSANCT - YUMA Remix</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Yosemite (Philip George Remix)</t>
+          <t>SACROSANCT (YUMA Remix)</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4.58</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="3">
@@ -500,21 +500,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Harry Hayes</t>
+          <t>KETTAMA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MissU2</t>
+          <t>Yosemite - Philip George Remix</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MissU2</t>
+          <t>Yosemite (Philip George Remix)</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3.67</v>
+        <v>4.58</v>
       </c>
     </row>
     <row r="4">
@@ -525,21 +525,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>salute</t>
+          <t>Harry Hayes</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jennifer - Extended</t>
+          <t>MissU2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>MissU2</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>5.49</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="5">
@@ -550,21 +550,21 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>What So Not</t>
+          <t>salute</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lights Go Out</t>
+          <t>Jennifer - Extended</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Lights Go Out</t>
+          <t>Jennifer</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4.01</v>
+        <v>5.49</v>
       </c>
     </row>
     <row r="6">
@@ -575,21 +575,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BL3SS</t>
+          <t>What So Not</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R 2 ME</t>
+          <t>Lights Go Out</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R 2 ME</t>
+          <t>Lights Go Out</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2.54</v>
+        <v>4.01</v>
       </c>
     </row>
     <row r="7">
@@ -600,21 +600,21 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Barry Can't Swim</t>
+          <t>BL3SS</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Kimpton</t>
+          <t>R 2 ME</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Kimpton</t>
+          <t>R 2 ME</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3.8</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="8">
@@ -625,21 +625,21 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Daniel Allan</t>
+          <t>Barry Can't Swim</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Something More</t>
+          <t>Kimpton</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Something More</t>
+          <t>Kimpton</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2.7</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="9">
@@ -650,21 +650,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LP Giobbi</t>
+          <t>Daniel Allan</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Love Come Through</t>
+          <t>Something More</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Love Come Through</t>
+          <t>Something More</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3.32</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="10">
@@ -675,21 +675,21 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Angrybaby</t>
+          <t>LP Giobbi</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>PUT IT DOWN</t>
+          <t>Love Come Through</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>PUT IT DOWN</t>
+          <t>Love Come Through</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2.17</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="11">
@@ -700,21 +700,21 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Conrad</t>
+          <t>Angrybaby</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>we stayed up all night</t>
+          <t>PUT IT DOWN</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>we stayed up all night</t>
+          <t>PUT IT DOWN</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>3.55</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="12">
@@ -725,21 +725,21 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EVAN GIIA</t>
+          <t>Conrad</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MUD MELODIES</t>
+          <t>we stayed up all night</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>STAMINA</t>
+          <t>we stayed up all night</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3.17</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="13">
@@ -750,21 +750,21 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ATTLAS</t>
+          <t>EVAN GIIA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>The One</t>
+          <t>MUD MELODIES</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>The One</t>
+          <t>STAMINA</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>3.26</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="14">
@@ -775,21 +775,21 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>gardenstate</t>
+          <t>ATTLAS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>The Best Part - Lost Prince Remix</t>
+          <t>The One</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>The Best Part (Remixes)</t>
+          <t>The One</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3.31</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="15">
@@ -800,17 +800,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Eli Brown</t>
+          <t>gardenstate</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Pulling Me Back</t>
+          <t>The Best Part - Lost Prince Remix</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Pulling Me Back</t>
+          <t>The Best Part (Remixes)</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -825,21 +825,21 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Tudor</t>
+          <t>Eli Brown</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bonfire</t>
+          <t>Pulling Me Back</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Bonfire</t>
+          <t>Pulling Me Back</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3.97</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="17">
@@ -850,21 +850,21 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>XANDRA</t>
+          <t>Tudor</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Feel Good - Punctual Remix</t>
+          <t>Bonfire</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Feel Good (Punctual Remix)</t>
+          <t>Bonfire</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>3.23</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="18">
@@ -875,21 +875,21 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Return Of The Jaded</t>
+          <t>XANDRA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Be The Reason - Club Mix</t>
+          <t>Feel Good - Punctual Remix</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Be The Reason (Club Mix)</t>
+          <t>Feel Good (Punctual Remix)</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>3.32</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="19">
@@ -900,21 +900,21 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Punctual</t>
+          <t>Return Of The Jaded</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>You're Not Alone - James Carter Remix</t>
+          <t>Be The Reason - Club Mix</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>You're Not Alone (James Carter Remix)</t>
+          <t>Be The Reason (Club Mix)</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>3.03</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="20">
@@ -925,21 +925,21 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>HÜMAN</t>
+          <t>Punctual</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Craving You</t>
+          <t>You're Not Alone - James Carter Remix</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Craving You</t>
+          <t>You're Not Alone (James Carter Remix)</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>4.45</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="21">
@@ -950,21 +950,21 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Volyri</t>
+          <t>HÜMAN</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Better Now</t>
+          <t>Craving You</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Better Now</t>
+          <t>Craving You</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>2.59</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="22">
@@ -975,21 +975,21 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>HKLMR</t>
+          <t>Volyri</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Serenity (Kin Le Max Remix)</t>
+          <t>Better Now</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Serenity (Kin Le Max Remix)</t>
+          <t>Better Now</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>2.72</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="23">
@@ -1000,21 +1000,21 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Calvin Harris</t>
+          <t>HKLMR</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Blessings</t>
+          <t>Serenity (Kin Le Max Remix)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Blessings</t>
+          <t>Serenity (Kin Le Max Remix)</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>3.66</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="24">
@@ -1025,21 +1025,21 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>KC Lights</t>
+          <t>Calvin Harris</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CHOOSE LOVE</t>
+          <t>Blessings</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>CHOOSE LOVE</t>
+          <t>Blessings</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2.78</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="25">
@@ -1050,21 +1050,21 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Spacey Jane</t>
+          <t>KC Lights</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Weightless</t>
+          <t>CHOOSE LOVE</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Sunlight</t>
+          <t>CHOOSE LOVE</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>4.18</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="26">
@@ -1080,16 +1080,16 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>Weightless</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>If That Makes Sense</t>
+          <t>Sunlight</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3.98</v>
+        <v>4.18</v>
       </c>
     </row>
     <row r="27">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ily the Most</t>
+          <t>August</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2.83</v>
+        <v>3.98</v>
       </c>
     </row>
     <row r="28">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Estimated Delivery</t>
+          <t>Ily the Most</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1139,7 +1139,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>3.42</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="29">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>The More That it Hurts</t>
+          <t>Estimated Delivery</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1164,7 +1164,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>3.03</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="30">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>So Much Taller</t>
+          <t>The More That it Hurts</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1189,7 +1189,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>3.34</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="31">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>I Can’t Afford to Lose You</t>
+          <t>So Much Taller</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1214,7 +1214,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>3.75</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="32">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>How to Kill Houseplants</t>
+          <t>I Can’t Afford to Lose You</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>3.48</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="33">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Impossible to Say</t>
+          <t>How to Kill Houseplants</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1264,7 +1264,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>3.53</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="34">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>All the Noise</t>
+          <t>Impossible to Say</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="35">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Whateverrrr</t>
+          <t>All the Noise</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1314,7 +1314,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2.97</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Through My Teeth</t>
+          <t>Whateverrrr</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>3.42</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="37">
@@ -1350,21 +1350,21 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Tchami</t>
+          <t>Spacey Jane</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Praise</t>
+          <t>Through My Teeth</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Year Zero</t>
+          <t>If That Makes Sense</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>3.5</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="38">
@@ -1375,17 +1375,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Goodboys</t>
+          <t>Tchami</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Blindspot</t>
+          <t>Praise</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Blindspot</t>
+          <t>Year Zero</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1400,21 +1400,21 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>RAYE</t>
+          <t>Goodboys</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Call On Me - KREAM Remix</t>
+          <t>Blindspot</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Call On Me (KREAM Remix)</t>
+          <t>Blindspot</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>3.68</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="40">
@@ -1425,21 +1425,21 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Three Drives On A Vinyl</t>
+          <t>RAYE</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Greece 2000 - KREAM Remix</t>
+          <t>Call On Me - KREAM Remix</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Greece 2000 (KREAM Remix)</t>
+          <t>Call On Me (KREAM Remix)</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>3.58</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="41">
@@ -1450,21 +1450,21 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>KREAM</t>
+          <t>Three Drives On A Vinyl</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Reverie</t>
+          <t>Greece 2000 - KREAM Remix</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Reverie</t>
+          <t>Greece 2000 (KREAM Remix)</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>3.48</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="42">
@@ -1480,16 +1480,16 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Manta</t>
+          <t>Reverie</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Manta</t>
+          <t>Reverie</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>4.12</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="43">
@@ -1500,21 +1500,21 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Koastle</t>
+          <t>KREAM</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Life (Can't Get Much Better)</t>
+          <t>Manta</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Life (Can't Get Much Better)</t>
+          <t>Manta</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>3.38</v>
+        <v>4.12</v>
       </c>
     </row>
     <row r="44">
@@ -1525,21 +1525,21 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Effemar</t>
+          <t>Koastle</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Needing Space</t>
+          <t>Life (Can't Get Much Better)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Needing Space</t>
+          <t>Life (Can't Get Much Better)</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>3.54</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="45">
@@ -1550,21 +1550,21 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ATRIP</t>
+          <t>Effemar</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HERZSCHLAG</t>
+          <t>Needing Space</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>KLUBPARTEI</t>
+          <t>Needing Space</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3.9</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="46">
@@ -1575,21 +1575,21 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>HotLap</t>
+          <t>ATRIP</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Set You Free</t>
+          <t>HERZSCHLAG</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Set You Free</t>
+          <t>KLUBPARTEI</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3.4</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="47">
@@ -1600,21 +1600,21 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Simon Doty</t>
+          <t>HotLap</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Tattoo</t>
+          <t>Set You Free</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Tattoo</t>
+          <t>Set You Free</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>3.65</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="48">
@@ -1625,21 +1625,21 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Tina Says</t>
+          <t>Simon Doty</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Barriers</t>
+          <t>Tattoo</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Barriers</t>
+          <t>Tattoo</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>3.24</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="49">
@@ -1650,21 +1650,21 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Tom Westy</t>
+          <t>Tina Says</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Remember Me</t>
+          <t>Barriers</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Remember Me</t>
+          <t>Barriers</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>3.14</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="50">
@@ -1675,21 +1675,21 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>JEWELS</t>
+          <t>Tom Westy</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>JETLAGGED</t>
+          <t>Remember Me</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>JETLAGGED</t>
+          <t>Remember Me</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>4.55</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="51">
@@ -1700,796 +1700,21 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Bad Friends</t>
+          <t>JEWELS</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Will U?</t>
+          <t>JETLAGGED</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Will U?</t>
+          <t>JETLAGGED</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>2.71</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Chazza Moo</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>You Don't See Me - Original Mix</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>You Don't See Me</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>salute</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Feel The Same</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Condition</t>
-        </is>
-      </c>
-      <c r="E53" t="n">
-        <v>4.42</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>A-Trak</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>My Own Way</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>My Own Way</t>
-        </is>
-      </c>
-      <c r="E54" t="n">
-        <v>2.35</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Belters Only</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>My Mind</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>My Mind</t>
-        </is>
-      </c>
-      <c r="E55" t="n">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Caroline Kole</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>What If - Dave Audé Remix</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>What If (The Remixes)</t>
-        </is>
-      </c>
-      <c r="E56" t="n">
-        <v>4.67</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>BROODS</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Peach - Golf Clap Remix</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Peach (Golf Clap Remix)</t>
-        </is>
-      </c>
-      <c r="E57" t="n">
-        <v>5.33</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Sebjak</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Yeah (Radio Edit)</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Yeah (Radio Edit)</t>
-        </is>
-      </c>
-      <c r="E58" t="n">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Higgo</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>I Just Wanna Dance</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>I Just Wanna Dance</t>
-        </is>
-      </c>
-      <c r="E59" t="n">
-        <v>2.73</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Oppidan</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>See Me</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>See Me</t>
-        </is>
-      </c>
-      <c r="E60" t="n">
-        <v>3.08</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>A-Trak</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Coming Home</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Coming Home</t>
-        </is>
-      </c>
-      <c r="E61" t="n">
-        <v>3.17</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Visions</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Visions</t>
-        </is>
-      </c>
-      <c r="E62" t="n">
-        <v>2.26</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Boston Bun</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Better Together</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Better Together</t>
-        </is>
-      </c>
-      <c r="E63" t="n">
-        <v>3.62</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Lo Lytes</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Losing My Mind - Niko The Kid Remix</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Losing My Mind (Niko The Kid Remix)</t>
-        </is>
-      </c>
-      <c r="E64" t="n">
-        <v>4.42</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>SG Lewis</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Hurting (feat. AlunaGeorge &amp; Sam Wise) - Conducta Remix</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Hurting (feat. AlunaGeorge &amp; Sam Wise) [Conducta Remix]</t>
-        </is>
-      </c>
-      <c r="E65" t="n">
-        <v>2.96</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>ANGELZ</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Inspheration</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Inspheration</t>
-        </is>
-      </c>
-      <c r="E66" t="n">
-        <v>5.01</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Oliver Dollar</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Pushing On</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Pushing On</t>
-        </is>
-      </c>
-      <c r="E67" t="n">
-        <v>2.72</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Wh0</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Soul Searcher</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Soul Searcher</t>
-        </is>
-      </c>
-      <c r="E68" t="n">
-        <v>3.14</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Punctual</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Repeating</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Repeating</t>
-        </is>
-      </c>
-      <c r="E69" t="n">
-        <v>2.46</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>BROHUG</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Stockholm</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Stockholm</t>
-        </is>
-      </c>
-      <c r="E70" t="n">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>ALYSS</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Pyramid</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Alchemy</t>
-        </is>
-      </c>
-      <c r="E71" t="n">
-        <v>3.89</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Panuma</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Don't Call Me</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Don't Call Me</t>
-        </is>
-      </c>
-      <c r="E72" t="n">
-        <v>4.34</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Thomas Garcia</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Feeling Dangerous</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Feeling Dangerous</t>
-        </is>
-      </c>
-      <c r="E73" t="n">
-        <v>3.66</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Topic</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Why Do You Lie To Me (feat. Lil Baby) - KC Lights Remix</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>Why Do You Lie To Me (feat. Lil Baby) [Remixes]</t>
-        </is>
-      </c>
-      <c r="E74" t="n">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>salute</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Peach</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>Peach</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
-        <v>5.76</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Nico de Andrea</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Woman</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Woman</t>
-        </is>
-      </c>
-      <c r="E76" t="n">
-        <v>3.57</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>PS1</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Life Goes On (feat. Alex Hosking) - KC Lights Remix</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Life Goes On (KC Lights Remix) (feat. Alex Hosking)</t>
-        </is>
-      </c>
-      <c r="E77" t="n">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Maeta</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Toxic (ft. Beam) - SWITCHDON Remix</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Habits (Remixes)</t>
-        </is>
-      </c>
-      <c r="E78" t="n">
-        <v>4.45</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Shadow Child</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>23 VIP</t>
-        </is>
-      </c>
-      <c r="E79" t="n">
-        <v>5.69</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>GRAACE</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>21st Century Love (Douvelle19 Remix)</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>21st Century Love (Douvelle19 Remix)</t>
-        </is>
-      </c>
-      <c r="E80" t="n">
-        <v>3.12</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Me &amp; George</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Slash</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Slash</t>
-        </is>
-      </c>
-      <c r="E81" t="n">
-        <v>3.72</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>Recursion Release Party Set</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>The Subculture</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Holdin’ On</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Holdin’ On</t>
-        </is>
-      </c>
-      <c r="E82" t="n">
-        <v>3.36</v>
+        <v>4.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
readme updates, made changes but ended up reverting back to previous commit
</commit_message>
<xml_diff>
--- a/backend/spotify_export.xlsx
+++ b/backend/spotify_export.xlsx
@@ -550,21 +550,21 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>salute</t>
+          <t>What So Not</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Jennifer - Extended</t>
+          <t>Lights Go Out</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>Lights Go Out</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>5.49</v>
+        <v>4.01</v>
       </c>
     </row>
     <row r="6">
@@ -575,21 +575,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>What So Not</t>
+          <t>BL3SS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Lights Go Out</t>
+          <t>R 2 ME</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Lights Go Out</t>
+          <t>R 2 ME</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>4.01</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="7">
@@ -600,21 +600,21 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BL3SS</t>
+          <t>Barry Can't Swim</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R 2 ME</t>
+          <t>Kimpton</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R 2 ME</t>
+          <t>Kimpton</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2.54</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="8">
@@ -625,21 +625,21 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Barry Can't Swim</t>
+          <t>Daniel Allan</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Kimpton</t>
+          <t>Something More</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Kimpton</t>
+          <t>Something More</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3.8</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="9">
@@ -650,21 +650,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Daniel Allan</t>
+          <t>Conrad.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Something More</t>
+          <t>we stayed up all night</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Something More</t>
+          <t>we stayed up all night</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2.7</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="10">
@@ -675,21 +675,21 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LP Giobbi</t>
+          <t>EVAN GIIA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Love Come Through</t>
+          <t>MUD MELODIES</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Love Come Through</t>
+          <t>STAMINA</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3.32</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="11">
@@ -700,21 +700,21 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Angrybaby</t>
+          <t>ATTLAS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PUT IT DOWN</t>
+          <t>The One</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PUT IT DOWN</t>
+          <t>The One</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2.17</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="12">
@@ -725,21 +725,21 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Conrad</t>
+          <t>gardenstate</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>we stayed up all night</t>
+          <t>The Best Part - Lost Prince Remix</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>we stayed up all night</t>
+          <t>The Best Part (Remixes)</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3.55</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="13">
@@ -750,21 +750,21 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>EVAN GIIA</t>
+          <t>Eli Brown</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MUD MELODIES</t>
+          <t>Pulling Me Back</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>STAMINA</t>
+          <t>Pulling Me Back</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>3.17</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="14">
@@ -775,21 +775,21 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ATTLAS</t>
+          <t>Tudor</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>The One</t>
+          <t>Bonfire</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>The One</t>
+          <t>Bonfire</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3.26</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="15">
@@ -800,21 +800,21 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>gardenstate</t>
+          <t>XANDRA</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>The Best Part - Lost Prince Remix</t>
+          <t>Feel Good - Punctual Remix</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>The Best Part (Remixes)</t>
+          <t>Feel Good (Punctual Remix)</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3.31</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="16">
@@ -825,21 +825,21 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Eli Brown</t>
+          <t>Return Of The Jaded</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Pulling Me Back</t>
+          <t>Be The Reason - Club Mix</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Pulling Me Back</t>
+          <t>Be The Reason (Club Mix)</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3.31</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="17">
@@ -850,21 +850,21 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tudor</t>
+          <t>Punctual</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bonfire</t>
+          <t>You're Not Alone - James Carter Remix</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Bonfire</t>
+          <t>You're Not Alone (James Carter Remix)</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>3.97</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="18">
@@ -875,21 +875,21 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>XANDRA</t>
+          <t>HÜMAN</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Feel Good - Punctual Remix</t>
+          <t>Craving You</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Feel Good (Punctual Remix)</t>
+          <t>Craving You</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>3.23</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="19">
@@ -900,21 +900,21 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Return Of The Jaded</t>
+          <t>Volyri</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Be The Reason - Club Mix</t>
+          <t>Better Now</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Be The Reason (Club Mix)</t>
+          <t>Better Now</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>3.32</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="20">
@@ -925,21 +925,21 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Punctual</t>
+          <t>HKLMR</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>You're Not Alone - James Carter Remix</t>
+          <t>Serenity (Kin Le Max Remix)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>You're Not Alone (James Carter Remix)</t>
+          <t>Serenity (Kin Le Max Remix)</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>3.03</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="21">
@@ -950,21 +950,21 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>HÜMAN</t>
+          <t>Calvin Harris</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Craving You</t>
+          <t>Blessings</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Craving You</t>
+          <t>Blessings</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>4.45</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="22">
@@ -975,21 +975,21 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Volyri</t>
+          <t>KC Lights</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Better Now</t>
+          <t>CHOOSE LOVE</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Better Now</t>
+          <t>CHOOSE LOVE</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>2.59</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="23">
@@ -1000,21 +1000,21 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>HKLMR</t>
+          <t>Spacey Jane</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Serenity (Kin Le Max Remix)</t>
+          <t>Weightless</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Serenity (Kin Le Max Remix)</t>
+          <t>Sunlight</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>2.72</v>
+        <v>4.18</v>
       </c>
     </row>
     <row r="24">
@@ -1025,21 +1025,21 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Calvin Harris</t>
+          <t>Spacey Jane</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Blessings</t>
+          <t>August</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Blessings</t>
+          <t>If That Makes Sense</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>3.66</v>
+        <v>3.98</v>
       </c>
     </row>
     <row r="25">
@@ -1050,21 +1050,21 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>KC Lights</t>
+          <t>Spacey Jane</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CHOOSE LOVE</t>
+          <t>Ily the Most</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>CHOOSE LOVE</t>
+          <t>If That Makes Sense</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>2.78</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="26">
@@ -1080,16 +1080,16 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Weightless</t>
+          <t>Estimated Delivery</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Sunlight</t>
+          <t>If That Makes Sense</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>4.18</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="27">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>The More That it Hurts</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>3.98</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="28">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ily the Most</t>
+          <t>So Much Taller</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1139,7 +1139,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>2.83</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="29">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Estimated Delivery</t>
+          <t>I Can’t Afford to Lose You</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1164,7 +1164,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>3.42</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="30">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>The More That it Hurts</t>
+          <t>How to Kill Houseplants</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1189,7 +1189,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>3.03</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="31">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>So Much Taller</t>
+          <t>Impossible to Say</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1214,7 +1214,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>3.34</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="32">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>I Can’t Afford to Lose You</t>
+          <t>All the Noise</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>3.75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>How to Kill Houseplants</t>
+          <t>Whateverrrr</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1264,7 +1264,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>3.48</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="34">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Impossible to Say</t>
+          <t>Through My Teeth</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>3.53</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="35">
@@ -1300,21 +1300,21 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Spacey Jane</t>
+          <t>Tchami</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>All the Noise</t>
+          <t>Praise</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>If That Makes Sense</t>
+          <t>Year Zero</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="36">
@@ -1325,21 +1325,21 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Spacey Jane</t>
+          <t>Goodboys</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Whateverrrr</t>
+          <t>Blindspot</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>If That Makes Sense</t>
+          <t>Blindspot</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2.97</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="37">
@@ -1350,21 +1350,21 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Spacey Jane</t>
+          <t>RAYE</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Through My Teeth</t>
+          <t>Call On Me - KREAM Remix</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>If That Makes Sense</t>
+          <t>Call On Me (KREAM Remix)</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>3.42</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="38">
@@ -1375,21 +1375,21 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tchami</t>
+          <t>Three Drives On A Vinyl</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Praise</t>
+          <t>Greece 2000 - KREAM Remix</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Year Zero</t>
+          <t>Greece 2000 (KREAM Remix)</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>3.5</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="39">
@@ -1400,21 +1400,21 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Goodboys</t>
+          <t>KREAM</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Blindspot</t>
+          <t>Reverie</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Blindspot</t>
+          <t>Reverie</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>3.5</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="40">
@@ -1425,21 +1425,21 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>RAYE</t>
+          <t>KREAM</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Call On Me - KREAM Remix</t>
+          <t>Manta</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Call On Me (KREAM Remix)</t>
+          <t>Manta</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>3.68</v>
+        <v>4.12</v>
       </c>
     </row>
     <row r="41">
@@ -1450,21 +1450,21 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Three Drives On A Vinyl</t>
+          <t>Koastle</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Greece 2000 - KREAM Remix</t>
+          <t>Life (Can't Get Much Better)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Greece 2000 (KREAM Remix)</t>
+          <t>Life (Can't Get Much Better)</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>3.58</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="42">
@@ -1475,21 +1475,21 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>KREAM</t>
+          <t>Effemar</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Reverie</t>
+          <t>Needing Space</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Reverie</t>
+          <t>Needing Space</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>3.48</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="43">
@@ -1500,21 +1500,21 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>KREAM</t>
+          <t>ATRIP</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Manta</t>
+          <t>HERZSCHLAG</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Manta</t>
+          <t>KLUBPARTEI</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>4.12</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="44">
@@ -1525,21 +1525,21 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Koastle</t>
+          <t>HotLap</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Life (Can't Get Much Better)</t>
+          <t>Set You Free</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Life (Can't Get Much Better)</t>
+          <t>Set You Free</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>3.38</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="45">
@@ -1550,21 +1550,21 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Effemar</t>
+          <t>Simon Doty</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Needing Space</t>
+          <t>Tattoo</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Needing Space</t>
+          <t>Tattoo</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3.54</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="46">
@@ -1575,21 +1575,21 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ATRIP</t>
+          <t>Tina Says</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>HERZSCHLAG</t>
+          <t>Barriers</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>KLUBPARTEI</t>
+          <t>Barriers</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3.9</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="47">
@@ -1600,21 +1600,21 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>HotLap</t>
+          <t>Tom Westy</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Set You Free</t>
+          <t>Remember Me</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Set You Free</t>
+          <t>Remember Me</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>3.4</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="48">
@@ -1625,21 +1625,21 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Simon Doty</t>
+          <t>JEWELS</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Tattoo</t>
+          <t>JETLAGGED</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Tattoo</t>
+          <t>JETLAGGED</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>3.65</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="49">
@@ -1650,21 +1650,21 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Tina Says</t>
+          <t>Bad Friends</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Barriers</t>
+          <t>Will U?</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Barriers</t>
+          <t>Will U?</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>3.24</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="50">
@@ -1675,21 +1675,21 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Tom Westy</t>
+          <t>Koastle</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Remember Me</t>
+          <t>Dr. Phil</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Remember Me</t>
+          <t>Dr. Phil</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>3.14</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="51">
@@ -1700,21 +1700,21 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>JEWELS</t>
+          <t>Koastle</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>JETLAGGED</t>
+          <t>Sabotage</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>JETLAGGED</t>
+          <t>Sabotage</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>4.55</v>
+        <v>3.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>